<commit_message>
Script updates for multisystem usage
</commit_message>
<xml_diff>
--- a/EEE/files/pair_matrix.xlsx
+++ b/EEE/files/pair_matrix.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bgrau\GitHub\git_ieeg_affect\scripts\oasis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bgrau\GitHub\ieeg_affect\EEE\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6F3BF195-6AAC-47A9-9AF6-295291E61A4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E786DF86-B39D-4285-8ADA-2B2614BC26C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="15466"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="15466" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pair_matrix" sheetId="1" r:id="rId1"/>
@@ -322,7 +322,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1156,11 +1156,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="E64" sqref="E64:E65"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -3323,10 +3323,10 @@
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A29">
-        <v>265</v>
+        <v>270</v>
       </c>
       <c r="B29" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C29" t="s">
         <v>35</v>
@@ -3338,72 +3338,72 @@
         <v>2</v>
       </c>
       <c r="F29" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G29">
-        <v>3.4313725490196099</v>
+        <v>5.9009900990099</v>
       </c>
       <c r="H29">
-        <v>1.74350167692974</v>
+        <v>0.94345058688888905</v>
       </c>
       <c r="I29">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J29">
-        <v>3.9306930693069302</v>
+        <v>4.1941747572815498</v>
       </c>
       <c r="K29">
-        <v>1.81249786616467</v>
+        <v>1.63334285167605</v>
       </c>
       <c r="L29">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="M29">
-        <v>3.511111111</v>
+        <v>5.6896551720000001</v>
       </c>
       <c r="N29">
-        <v>1.6871468949999999</v>
+        <v>0.94045335399999996</v>
       </c>
       <c r="O29">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="P29">
-        <v>3.4107142860000002</v>
+        <v>6.1860465119999999</v>
       </c>
       <c r="Q29">
-        <v>1.786584204</v>
+        <v>0.87982178799999999</v>
       </c>
       <c r="R29">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="S29">
-        <v>3.7959183670000001</v>
+        <v>4.0816326529999998</v>
       </c>
       <c r="T29">
-        <v>1.881705696</v>
+        <v>1.5115766420000001</v>
       </c>
       <c r="U29">
         <v>49</v>
       </c>
       <c r="V29">
-        <v>4.057692308</v>
+        <v>4.2830188680000001</v>
       </c>
       <c r="W29">
-        <v>1.7535785429999999</v>
+        <v>1.758248238</v>
       </c>
       <c r="X29">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="Y29">
-        <v>0.100396824999999</v>
+        <v>0.49639133999999902</v>
       </c>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A30">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="B30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C30" t="s">
         <v>35</v>
@@ -3415,64 +3415,64 @@
         <v>1</v>
       </c>
       <c r="F30" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="G30">
-        <v>5.9009900990099</v>
+        <v>3.4313725490196099</v>
       </c>
       <c r="H30">
-        <v>0.94345058688888905</v>
+        <v>1.74350167692974</v>
       </c>
       <c r="I30">
+        <v>102</v>
+      </c>
+      <c r="J30">
+        <v>3.9306930693069302</v>
+      </c>
+      <c r="K30">
+        <v>1.81249786616467</v>
+      </c>
+      <c r="L30">
         <v>101</v>
       </c>
-      <c r="J30">
-        <v>4.1941747572815498</v>
-      </c>
-      <c r="K30">
-        <v>1.63334285167605</v>
-      </c>
-      <c r="L30">
-        <v>103</v>
-      </c>
       <c r="M30">
-        <v>5.6896551720000001</v>
+        <v>3.511111111</v>
       </c>
       <c r="N30">
-        <v>0.94045335399999996</v>
+        <v>1.6871468949999999</v>
       </c>
       <c r="O30">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="P30">
-        <v>6.1860465119999999</v>
+        <v>3.4107142860000002</v>
       </c>
       <c r="Q30">
-        <v>0.87982178799999999</v>
+        <v>1.786584204</v>
       </c>
       <c r="R30">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="S30">
-        <v>4.0816326529999998</v>
+        <v>3.7959183670000001</v>
       </c>
       <c r="T30">
-        <v>1.5115766420000001</v>
+        <v>1.881705696</v>
       </c>
       <c r="U30">
         <v>49</v>
       </c>
       <c r="V30">
-        <v>4.2830188680000001</v>
+        <v>4.057692308</v>
       </c>
       <c r="W30">
-        <v>1.758248238</v>
+        <v>1.7535785429999999</v>
       </c>
       <c r="X30">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Y30">
-        <v>0.49639133999999902</v>
+        <v>0.100396824999999</v>
       </c>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.5">

</xml_diff>